<commit_message>
Products Catalog > Products: rename 'קטגוריה' to 'תת קטגוריה' and load combobox options from categories.json
</commit_message>
<xml_diff>
--- a/קובץ מוצרים.xlsx
+++ b/קובץ מוצרים.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -930,6 +930,96 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>04 pants futer pok KOFIKO(2).PDS</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>מכנס ארוך מולי ילדים חורף 25-26</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>t-shirt long sleeve (bk+4.5cm).PDS</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>חולצת ילדים ש.א מולי 25\26</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>026 Baby bodysuit amrican color loong sleeve new.PDS</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>בגד גוף צווארון אמריקאי</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>04 pants futer pok KOFIKO (2).PDS</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>מכנס ארוך מולי ילדים חורף 25-26</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>24-02 gatkes baby.PDS</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>מכנס תינוק מולי חורף 25-26</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>04 pants futer pof KOFIKO (2).PDS</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>מכנס ארוך מולי ילדים חורף 25-26</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Delivery Note: add Main Category selector and dynamic field visibility; Products Catalog: make subcategory optional; new Stickers tab mixin and integration; minor UI polish
</commit_message>
<xml_diff>
--- a/קובץ מוצרים.xlsx
+++ b/קובץ מוצרים.xlsx
@@ -933,12 +933,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04 pants futer pok KOFIKO(2).PDS</t>
+          <t>t-shirt long sleeve (bk+4.5cm).PDS</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>מכנס ארוך מולי ילדים חורף 25-26</t>
+          <t>חולצת ילדים ש.א מולי 25\26</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -948,12 +948,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>t-shirt long sleeve (bk+4.5cm).PDS</t>
+          <t>04 pants futer pok KOFIKO (2).PDS</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>חולצת ילדים ש.א מולי 25\26</t>
+          <t>מכנס ארוך מולי ילדים חורף 25-26</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -963,12 +963,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>026 Baby bodysuit amrican color loong sleeve new.PDS</t>
+          <t>24-02 gatkes baby.PDS</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>בגד גוף צווארון אמריקאי</t>
+          <t>מכנס תינוק מולי חורף 25-26</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -978,7 +978,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04 pants futer pok KOFIKO (2).PDS</t>
+          <t>04 pants futer pof KOFIKO (2).PDS</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -993,12 +993,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>24-02 gatkes baby.PDS</t>
+          <t>026  Baby bodysuit amrican color loong sleeve  new.PDS</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>מכנס תינוק מולי חורף 25-26</t>
+          <t>בגד גוף צווארון אמריקאי</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1008,12 +1008,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04 pants futer pof KOFIKO (2).PDS</t>
+          <t>25-01 dress singel fabric (8).PDS</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>מכנס ארוך מולי ילדים חורף 25-26</t>
+          <t>שמלה ש.א מולי25-26</t>
         </is>
       </c>
       <c r="C39" t="n">

</xml_diff>

<commit_message>
Update drawings data and project files
</commit_message>
<xml_diff>
--- a/קובץ מוצרים.xlsx
+++ b/קובץ מוצרים.xlsx
@@ -743,7 +743,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>גופוית פלנל</t>
+          <t>גופיות פלנל</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -758,7 +758,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>גופוית פלנל</t>
+          <t>גופיות פלנל</t>
         </is>
       </c>
       <c r="C22" t="n">

</xml_diff>

<commit_message>
Update data files: drawings, fabrics shipments and products
</commit_message>
<xml_diff>
--- a/קובץ מוצרים.xlsx
+++ b/קובץ מוצרים.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1035,6 +1035,21 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>026  Baby bodysuit short sleeve 2025 6-9,9-12.PDS</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>בגד גוף קצר כולל מידה6-9 9-12</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>